<commit_message>
fixed fertilizer calcs, works for siskiyou now
</commit_message>
<xml_diff>
--- a/R/data_raw/greet_ag-chemicals.xlsx
+++ b/R/data_raw/greet_ag-chemicals.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_raw\greet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4FA939-DFC7-4A29-8A9F-DB75F1E201CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC95E110-5D1B-4BC8-9D6C-37685DEA43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9625B5A-585C-42B4-8F9D-D6C6CCB243F3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D9625B5A-585C-42B4-8F9D-D6C6CCB243F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fert-4chems" sheetId="1" r:id="rId1"/>
+    <sheet name="fert-prods" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
+    <definedName name="Ammonia_Prod_NGFeedShare">#REF!</definedName>
+    <definedName name="FuelSpec_EtOH_Density">[2]Fuel_Specs!$E$32</definedName>
+    <definedName name="kg2g">[2]Fuel_Specs!$C$181</definedName>
+    <definedName name="kg2T">[2]Fuel_Specs!$C$185</definedName>
+    <definedName name="kWh2BTU">[2]Fuel_Specs!$F$200</definedName>
+    <definedName name="lb2g">[2]Fuel_Specs!$E$181</definedName>
+    <definedName name="MJ2kWh">[2]Fuel_Specs!$D$199</definedName>
+    <definedName name="MJ2mmBTU">[2]Fuel_Specs!$D$201</definedName>
     <definedName name="T2g">[1]Fuel_Specs!$F$181</definedName>
+    <definedName name="T2lb">[2]Fuel_Specs!$F$184</definedName>
+    <definedName name="Wh2BTU">[2]Fuel_Specs!$E$200</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>5) Summary of Energy Use, Water Consumption, and Emissions of Agricultural Chemicals: per gram</t>
   </si>
@@ -129,6 +141,84 @@
   </si>
   <si>
     <t>AgInputs tab, starts at line 129</t>
+  </si>
+  <si>
+    <t>Phosphoric Acid (per ton of P2O5 product)</t>
+  </si>
+  <si>
+    <t>Ammonium Chloride (NH4Cl)</t>
+  </si>
+  <si>
+    <t>Monoammonium Phosphate (NH4H2PO4)</t>
+  </si>
+  <si>
+    <t>Ammonium Sulfate ((NH4)2SO4)</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>Ammonium Nitrate</t>
+  </si>
+  <si>
+    <t>Sulfuric Acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Total Energy</t>
+  </si>
+  <si>
+    <t>4) Calculation of Energy Use, Water Consumption, and Emissions of Fertilizer Production: Production Processes and Feedstock-Related Activities</t>
+  </si>
+  <si>
+    <t>Urea-Ammonium Nitrate Solution</t>
+  </si>
+  <si>
+    <t>Potash</t>
+  </si>
+  <si>
+    <t>Sodium Nitrate (NaNO3)</t>
+  </si>
+  <si>
+    <t>Potassium Nitrate (KNO3)</t>
+  </si>
+  <si>
+    <t>Calcium Nitrate (Ca(NO3)2)</t>
+  </si>
+  <si>
+    <t>Calcium Nitrate (Ca(NO3)2.4H2O)</t>
+  </si>
+  <si>
+    <t>Potassium Phosphates (K2HPO4)</t>
+  </si>
+  <si>
+    <t>Potassium Phosphates (K2HPO4.3H2O)</t>
+  </si>
+  <si>
+    <t>Potassium Phosphates (KH2PO4)</t>
+  </si>
+  <si>
+    <t>Diammonium Phosphate ((NH4)2HPO4)</t>
+  </si>
+  <si>
+    <t>Potassium Sulfate (K2SO4)</t>
+  </si>
+  <si>
+    <t>Superphosphate (Ca(H2PO4)2 + 2CaSO4)</t>
+  </si>
+  <si>
+    <t>Triple Superphosphate (Ca(H2PO4)2)</t>
+  </si>
+  <si>
+    <t>Triple Superphosphate (Ca(H2PO4)2.H2O)</t>
+  </si>
+  <si>
+    <t>Energy Use: mmBtu/ton</t>
+  </si>
+  <si>
+    <t>AgInputs tab, starts at line 94</t>
   </si>
 </sst>
 </file>
@@ -425,8 +515,152 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Overview"/>
+      <sheetName val="Inputs"/>
+      <sheetName val="Results"/>
+      <sheetName val="H2_User_Inputs"/>
+      <sheetName val="Petroleum"/>
+      <sheetName val="Co_processing"/>
+      <sheetName val="NG"/>
+      <sheetName val="MeOH_FTD"/>
+      <sheetName val="EtOH"/>
+      <sheetName val="Electric"/>
+      <sheetName val="Bio_electricity"/>
+      <sheetName val="Hydrogen"/>
+      <sheetName val="BioOil"/>
+      <sheetName val="Algae"/>
+      <sheetName val="Macroalgae"/>
+      <sheetName val="Waste"/>
+      <sheetName val="RNG"/>
+      <sheetName val="Pyrolysis_IDL"/>
+      <sheetName val="IBR"/>
+      <sheetName val="PUP_conversion"/>
+      <sheetName val="CESA"/>
+      <sheetName val="E_fuel"/>
+      <sheetName val="Fuel_Prod_TS"/>
+      <sheetName val="EF_TS"/>
+      <sheetName val="AgMining_EF_TS"/>
+      <sheetName val="EF"/>
+      <sheetName val="WCF"/>
+      <sheetName val="Fuel_Specs"/>
+      <sheetName val="Car_TS"/>
+      <sheetName val="LDT1_TS"/>
+      <sheetName val="LDT2_TS"/>
+      <sheetName val="Vehicles"/>
+      <sheetName val="Urban_Shares"/>
+      <sheetName val="Compression"/>
+      <sheetName val="Coal"/>
+      <sheetName val="T&amp;D_Flowcharts"/>
+      <sheetName val="T&amp;D"/>
+      <sheetName val="Uranium"/>
+      <sheetName val="ASU"/>
+      <sheetName val="Ag_Inputs"/>
+      <sheetName val="Enzymes_Yeast"/>
+      <sheetName val="Pretreatment"/>
+      <sheetName val="Catalyst"/>
+      <sheetName val="Steam_Cracking"/>
+      <sheetName val="Chemicals"/>
+      <sheetName val="Plastics"/>
+      <sheetName val="Animal_Feed"/>
+      <sheetName val="EtOH-Diesel Additives"/>
+      <sheetName val="OilGasCoalInfra"/>
+      <sheetName val="ElecInfra"/>
+      <sheetName val="Woody"/>
+      <sheetName val="HDV_TS"/>
+      <sheetName val="HDV_WTW"/>
+      <sheetName val="JetFuel_WTP"/>
+      <sheetName val="JetFuel_PTWa"/>
+      <sheetName val="JetFuel_WTWa"/>
+      <sheetName val="Rail_PTW"/>
+      <sheetName val="Rail_WTW"/>
+      <sheetName val="Marine_WTH"/>
+      <sheetName val="Dist_Spec"/>
+      <sheetName val="Forecast_Specs"/>
+      <sheetName val="Forecast_Deleted"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1">
+        <row r="181">
+          <cell r="F181">
+            <v>907184.74</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Overview"/>
       <sheetName val="Inputs"/>
@@ -520,9 +754,45 @@
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27">
+        <row r="32">
+          <cell r="E32">
+            <v>2988</v>
+          </cell>
+        </row>
         <row r="181">
-          <cell r="F181">
-            <v>907184.74</v>
+          <cell r="C181">
+            <v>1000</v>
+          </cell>
+          <cell r="E181">
+            <v>453.59237000000002</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="F184">
+            <v>2000</v>
+          </cell>
+        </row>
+        <row r="185">
+          <cell r="C185">
+            <v>1.1023113109243879E-3</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="D199">
+            <v>0.27777777777777779</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="E200">
+            <v>3.4121416416012482</v>
+          </cell>
+          <cell r="F200">
+            <v>3412.141641601248</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="D201">
+            <v>9.4781712266701326E-4</v>
           </cell>
         </row>
       </sheetData>
@@ -563,6 +833,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -864,28 +1138,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849F16D3-B719-444B-988E-5FFE4327B9F7}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -906,7 +1180,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>4</v>
@@ -945,7 +1219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -986,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
@@ -995,7 +1269,7 @@
       <c r="J10" s="15"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1292,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1315,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1064,7 +1338,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1087,7 +1361,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1384,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1133,7 +1407,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1156,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1447,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="23"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1214,7 +1488,7 @@
         <v>213.33062067431146</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1529,7 @@
         <v>200.92487387036792</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1296,7 +1570,7 @@
         <v>21.068475437804288</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1337,7 +1611,7 @@
         <v>76.333834859502645</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>23</v>
       </c>
@@ -1376,6 +1650,483 @@
       </c>
       <c r="M23" s="30">
         <v>103.52256357306098</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E8F256-A12F-4B15-8599-465CD3B4E118}">
+  <dimension ref="A1:X11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="131.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" t="s">
+        <v>50</v>
+      </c>
+      <c r="V6" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" t="s">
+        <v>52</v>
+      </c>
+      <c r="X6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>32.391121261642439</v>
+      </c>
+      <c r="C7">
+        <v>24.591687743504753</v>
+      </c>
+      <c r="D7">
+        <v>16.74397064653116</v>
+      </c>
+      <c r="E7">
+        <v>55.466444848608532</v>
+      </c>
+      <c r="F7">
+        <v>0.51804777656533729</v>
+      </c>
+      <c r="G7">
+        <v>19.009994883486311</v>
+      </c>
+      <c r="H7">
+        <v>7.0844382213010455</v>
+      </c>
+      <c r="I7">
+        <v>0.10811671185723913</v>
+      </c>
+      <c r="J7">
+        <v>7.1730248495675477</v>
+      </c>
+      <c r="K7">
+        <v>5.7653551185388547</v>
+      </c>
+      <c r="L7">
+        <v>8.6144483374121421</v>
+      </c>
+      <c r="M7">
+        <v>8.1809256024868908</v>
+      </c>
+      <c r="N7">
+        <v>5.8578702837741181</v>
+      </c>
+      <c r="O7">
+        <v>27.05426636717835</v>
+      </c>
+      <c r="P7">
+        <v>20.785172437864393</v>
+      </c>
+      <c r="Q7">
+        <v>24.485385721124434</v>
+      </c>
+      <c r="R7">
+        <v>19.79518494263769</v>
+      </c>
+      <c r="S7">
+        <v>21.31762639942735</v>
+      </c>
+      <c r="T7">
+        <v>8.1604548581796941</v>
+      </c>
+      <c r="U7">
+        <v>3.4777988069752492</v>
+      </c>
+      <c r="V7">
+        <v>13.321827005225181</v>
+      </c>
+      <c r="W7">
+        <v>12.410386213365415</v>
+      </c>
+      <c r="X7">
+        <v>9.1561854031965932</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>32.288870296409321</v>
+      </c>
+      <c r="C8">
+        <v>24.331948514884047</v>
+      </c>
+      <c r="D8">
+        <v>16.591035604983531</v>
+      </c>
+      <c r="E8">
+        <v>54.74090575706704</v>
+      </c>
+      <c r="F8">
+        <v>0.48833806356676618</v>
+      </c>
+      <c r="G8">
+        <v>17.671898926224138</v>
+      </c>
+      <c r="H8">
+        <v>6.369685052570877</v>
+      </c>
+      <c r="I8">
+        <v>0.10748818051358598</v>
+      </c>
+      <c r="J8">
+        <v>6.457877952842896</v>
+      </c>
+      <c r="K8">
+        <v>5.6912713260185894</v>
+      </c>
+      <c r="L8">
+        <v>8.2063685484556625</v>
+      </c>
+      <c r="M8">
+        <v>8.1444875931929026</v>
+      </c>
+      <c r="N8">
+        <v>5.8316832678193276</v>
+      </c>
+      <c r="O8">
+        <v>23.459029539909896</v>
+      </c>
+      <c r="P8">
+        <v>18.040258980837269</v>
+      </c>
+      <c r="Q8">
+        <v>21.679008992975145</v>
+      </c>
+      <c r="R8">
+        <v>18.687443602562713</v>
+      </c>
+      <c r="S8">
+        <v>20.28733537435004</v>
+      </c>
+      <c r="T8">
+        <v>7.3360918370343944</v>
+      </c>
+      <c r="U8">
+        <v>3.2785706366861707</v>
+      </c>
+      <c r="V8">
+        <v>12.40367752143464</v>
+      </c>
+      <c r="W8">
+        <v>11.557653137613039</v>
+      </c>
+      <c r="X8">
+        <v>9.1056625412490835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>0.17369656550357981</v>
+      </c>
+      <c r="C9">
+        <v>0.44154504714961001</v>
+      </c>
+      <c r="D9">
+        <v>0.25973783539008549</v>
+      </c>
+      <c r="E9">
+        <v>1.2324080087483187</v>
+      </c>
+      <c r="F9">
+        <v>5.0454899659998068E-2</v>
+      </c>
+      <c r="G9">
+        <v>2.2749511028304705</v>
+      </c>
+      <c r="H9">
+        <v>1.215444022996707</v>
+      </c>
+      <c r="I9">
+        <v>4.5178283611293016E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.2160893421124765</v>
+      </c>
+      <c r="K9">
+        <v>0.23633690237898994</v>
+      </c>
+      <c r="L9">
+        <v>0.69378877444785847</v>
+      </c>
+      <c r="M9">
+        <v>6.3794459673292156E-2</v>
+      </c>
+      <c r="N9">
+        <v>4.5758140812928172E-2</v>
+      </c>
+      <c r="O9">
+        <v>6.1156748267043923</v>
+      </c>
+      <c r="P9">
+        <v>4.6691972426698243</v>
+      </c>
+      <c r="Q9">
+        <v>4.7733283442923069</v>
+      </c>
+      <c r="R9">
+        <v>1.8833426450073891</v>
+      </c>
+      <c r="S9">
+        <v>1.7516569662492045</v>
+      </c>
+      <c r="T9">
+        <v>1.4018319847920364</v>
+      </c>
+      <c r="U9">
+        <v>0.33858028416436797</v>
+      </c>
+      <c r="V9">
+        <v>1.5609463476000311</v>
+      </c>
+      <c r="W9">
+        <v>1.4497213053471278</v>
+      </c>
+      <c r="X9">
+        <v>8.5707387648597103E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>31.189125924490845</v>
+      </c>
+      <c r="C10">
+        <v>22.591536502213319</v>
+      </c>
+      <c r="D10">
+        <v>14.757243972478964</v>
+      </c>
+      <c r="E10">
+        <v>46.655092326072328</v>
+      </c>
+      <c r="F10">
+        <v>0.12314767302722145</v>
+      </c>
+      <c r="G10">
+        <v>9.5250058125836468</v>
+      </c>
+      <c r="H10">
+        <v>2.8876138679217931</v>
+      </c>
+      <c r="I10">
+        <v>1.108271003684648E-2</v>
+      </c>
+      <c r="J10">
+        <v>2.8938749780974882</v>
+      </c>
+      <c r="K10">
+        <v>4.4951863007671022</v>
+      </c>
+      <c r="L10">
+        <v>5.7079512429676909</v>
+      </c>
+      <c r="M10">
+        <v>7.010078378117746</v>
+      </c>
+      <c r="N10">
+        <v>4.8888459671605435</v>
+      </c>
+      <c r="O10">
+        <v>12.363710476902725</v>
+      </c>
+      <c r="P10">
+        <v>9.4512834889903434</v>
+      </c>
+      <c r="Q10">
+        <v>11.509628347628507</v>
+      </c>
+      <c r="R10">
+        <v>12.031428086135186</v>
+      </c>
+      <c r="S10">
+        <v>14.072266931810429</v>
+      </c>
+      <c r="T10">
+        <v>3.3049937130030025</v>
+      </c>
+      <c r="U10">
+        <v>1.6176157735303769</v>
+      </c>
+      <c r="V10">
+        <v>6.6921608553902407</v>
+      </c>
+      <c r="W10">
+        <v>6.2181246802382102</v>
+      </c>
+      <c r="X10">
+        <v>8.1750464576603896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>0.92604780641489315</v>
+      </c>
+      <c r="C11">
+        <v>1.2988669655211178</v>
+      </c>
+      <c r="D11">
+        <v>1.5740537971144795</v>
+      </c>
+      <c r="E11">
+        <v>6.8534054222463983</v>
+      </c>
+      <c r="F11">
+        <v>0.31473549087954666</v>
+      </c>
+      <c r="G11">
+        <v>5.8719420108100211</v>
+      </c>
+      <c r="H11">
+        <v>2.2666271616523765</v>
+      </c>
+      <c r="I11">
+        <v>9.1887642115610194E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.3479136326329315</v>
+      </c>
+      <c r="K11">
+        <v>0.95974812287249756</v>
+      </c>
+      <c r="L11">
+        <v>1.8046285310401133</v>
+      </c>
+      <c r="M11">
+        <v>1.0706147554018637</v>
+      </c>
+      <c r="N11">
+        <v>0.89707915984585562</v>
+      </c>
+      <c r="O11">
+        <v>4.9796442363027777</v>
+      </c>
+      <c r="P11">
+        <v>3.9197782491771007</v>
+      </c>
+      <c r="Q11">
+        <v>5.3960523010543318</v>
+      </c>
+      <c r="R11">
+        <v>4.7726728714201387</v>
+      </c>
+      <c r="S11">
+        <v>4.463411476290406</v>
+      </c>
+      <c r="T11">
+        <v>2.629266139239355</v>
+      </c>
+      <c r="U11">
+        <v>1.3223745789914259</v>
+      </c>
+      <c r="V11">
+        <v>4.150570318444367</v>
+      </c>
+      <c r="W11">
+        <v>3.8898071520277022</v>
+      </c>
+      <c r="X11">
+        <v>0.84490869594009621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>